<commit_message>
[add]: seperate excel sheet created for graphs
</commit_message>
<xml_diff>
--- a/CURRENT WORK/SALT WORK - CODES/N = 4/Li2SO4 - Done/Test_excelsheet for Li2SO4 n=4.xlsx
+++ b/CURRENT WORK/SALT WORK - CODES/N = 4/Li2SO4 - Done/Test_excelsheet for Li2SO4 n=4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhanu\OneDrive\Desktop\Final-Year-Project\CURRENT WORK\SALT WORK - CODES\N = 4\Li2SO4 - Done\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E9103A-5EF2-4003-9A4E-02F16453076F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80370323-39F8-4F68-9ADA-068015921FD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="657" firstSheet="1" activeTab="1" xr2:uid="{86974002-CAD5-4FCC-AF77-EBAA345E04BF}"/>
   </bookViews>
@@ -746,6 +746,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Data Points</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -1086,6 +1089,127 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Parity Line</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="15875" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'For finding 12 unknows'!$AW$9:$AW$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99999999999999989</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0999999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'For finding 12 unknows'!$AX$9:$AX$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99999999999999989</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0999999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5FFB-4274-B070-F2AB6D3AFE70}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1102,7 +1226,6 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
-          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1156,8 +1279,8 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1188,7 +1311,7 @@
         <c:crossAx val="1501985871"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="0.2"/>
+        <c:minorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="1501985871"/>
@@ -1248,8 +1371,8 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1280,6 +1403,7 @@
         <c:crossAx val="1240791008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:minorUnit val="0.1"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1337,7 +1461,6 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
-  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -4163,8 +4286,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18347475982977859"/>
-          <c:y val="0.8771929824561403"/>
+          <c:x val="0.18641458333333333"/>
+          <c:y val="0.90659120370370372"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4223,23 +4346,8 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="216"/>
-                <c:pt idx="0">
-                  <c:v>8.5834900000000006E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.14215900000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.14127400000000001</c:v>
-                </c:pt>
                 <c:pt idx="3">
                   <c:v>0.14638200000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.13661799999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.6268300000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>7.7306899999999998E-2</c:v>
@@ -4403,23 +4511,8 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="216"/>
-                <c:pt idx="0">
-                  <c:v>260</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>261</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>262</c:v>
-                </c:pt>
                 <c:pt idx="3">
                   <c:v>263</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>264</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>265</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>266</c:v>
@@ -4885,7 +4978,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-IN"/>
-                  <a:t>Ø</a:t>
+                  <a:t>Volume Fraction</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4917,8 +5010,8 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -4950,11 +5043,13 @@
         <c:crossAx val="472873184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:minorUnit val="2.5000000000000005E-2"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="472873184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="200"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -5008,8 +5103,8 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -5040,6 +5135,7 @@
         <c:crossAx val="596408272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:minorUnit val="25"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -9139,16 +9235,16 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>48</xdr:col>
-      <xdr:colOff>210120</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>23164</xdr:rowOff>
+      <xdr:col>52</xdr:col>
+      <xdr:colOff>453960</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>167944</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>55</xdr:col>
-      <xdr:colOff>262920</xdr:colOff>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>506760</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>144544</xdr:rowOff>
+      <xdr:rowOff>106444</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9175,249 +9271,10 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>49</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>51</xdr:col>
-      <xdr:colOff>335280</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="TextBox 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D16A807-0EB1-4658-B784-B5D3A9A58B3C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="37536120" y="2339340"/>
-          <a:ext cx="1234440" cy="449580"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-IN" sz="1100"/>
-            <a:t>         Data Points</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-IN" sz="1100" baseline="0"/>
-            <a:t>         Parity Line</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-IN" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>49</xdr:col>
-      <xdr:colOff>464820</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>49</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Flowchart: Connector 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91EC19DE-FA94-4234-908F-234D68878487}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="37680900" y="2438400"/>
-          <a:ext cx="106680" cy="114300"/>
-        </a:xfrm>
-        <a:prstGeom prst="flowChartConnector">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="C00000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-IN" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>49</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>50</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="9" name="Straight Connector 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74CE5646-EDF4-401D-BD32-9EC2E8C039ED}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="37642800" y="2667000"/>
-          <a:ext cx="213360" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.14363</cdr:x>
-      <cdr:y>0.05828</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.95746</cdr:x>
-      <cdr:y>0.7196</cdr:y>
-    </cdr:to>
-    <cdr:cxnSp macro="">
-      <cdr:nvCxnSpPr>
-        <cdr:cNvPr id="3" name="Straight Connector 2">
-          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71D34628-9E02-ED97-3D76-9F236D61FA8A}"/>
-            </a:ext>
-          </a:extLst>
-        </cdr:cNvPr>
-        <cdr:cNvCxnSpPr/>
-      </cdr:nvCxnSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipV="1">
-          <a:off x="620460" y="251755"/>
-          <a:ext cx="3515777" cy="2856901"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-      </cdr:spPr>
-      <cdr:style>
-        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </cdr:style>
-    </cdr:cxnSp>
-  </cdr:relSizeAnchor>
-</c:userShapes>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -9458,7 +9315,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -9573,7 +9430,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -10983,10 +10840,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88D00978-96AD-440F-AA3F-9C948C561128}">
-  <dimension ref="A1:AU84"/>
+  <dimension ref="A1:AX84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BE24" sqref="BE24"/>
+    <sheetView tabSelected="1" topLeftCell="AR7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BL12" sqref="BL12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11022,7 +10879,7 @@
     <col min="44" max="44" width="13.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:50" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B1" s="4" t="s">
         <v>33</v>
       </c>
@@ -11041,7 +10898,7 @@
       <c r="AG1"/>
       <c r="AL1"/>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
       <c r="H2"/>
       <c r="K2" s="6" t="s">
         <v>8</v>
@@ -11064,7 +10921,7 @@
       <c r="AG2" s="1"/>
       <c r="AL2"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
       <c r="H3"/>
       <c r="K3" s="6" t="s">
         <v>9</v>
@@ -11087,7 +10944,7 @@
       <c r="AG3" s="1"/>
       <c r="AL3"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
       <c r="H4"/>
       <c r="R4"/>
       <c r="V4"/>
@@ -11104,7 +10961,7 @@
       <c r="AG4" s="1"/>
       <c r="AL4"/>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
       <c r="H5"/>
       <c r="R5"/>
       <c r="V5"/>
@@ -11113,7 +10970,7 @@
       <c r="AG5"/>
       <c r="AL5"/>
     </row>
-    <row r="6" spans="1:47" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:50" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -11223,7 +11080,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1.0960399999999999</v>
       </c>
@@ -11359,7 +11216,7 @@
         <v>0.74580000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1.0263</v>
       </c>
@@ -11491,7 +11348,7 @@
         <v>0.74409999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>0.94349000000000005</v>
       </c>
@@ -11628,8 +11485,14 @@
       <c r="AR9" s="1">
         <v>0.74250000000000005</v>
       </c>
-    </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AW9">
+        <v>0</v>
+      </c>
+      <c r="AX9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>0.94342000000000004</v>
       </c>
@@ -11766,8 +11629,16 @@
       <c r="AR10" s="1">
         <v>0.74239999999999995</v>
       </c>
-    </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AW10">
+        <f>AW9+0.1</f>
+        <v>0.1</v>
+      </c>
+      <c r="AX10">
+        <f>AX9+0.1</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>0.43031000000000003</v>
       </c>
@@ -11904,8 +11775,16 @@
       <c r="AR11" s="1">
         <v>0.74760000000000004</v>
       </c>
-    </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AW11">
+        <f t="shared" ref="AW11:AX28" si="28">AW10+0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="AX11">
+        <f t="shared" si="28"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>0.42624000000000001</v>
       </c>
@@ -12042,8 +11921,16 @@
       <c r="AR12" s="1">
         <v>0.74939999999999996</v>
       </c>
-    </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AW12">
+        <f t="shared" si="28"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="AX12">
+        <f t="shared" si="28"/>
+        <v>0.30000000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>0.15548000000000001</v>
       </c>
@@ -12180,8 +12067,16 @@
       <c r="AR13" s="1">
         <v>0.7833</v>
       </c>
-    </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AW13">
+        <f t="shared" si="28"/>
+        <v>0.4</v>
+      </c>
+      <c r="AX13">
+        <f t="shared" si="28"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>0.1148</v>
       </c>
@@ -12318,8 +12213,16 @@
       <c r="AR14" s="1">
         <v>0.79339999999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AW14">
+        <f t="shared" si="28"/>
+        <v>0.5</v>
+      </c>
+      <c r="AX14">
+        <f t="shared" si="28"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>2.7969200000000001</v>
       </c>
@@ -12457,15 +12360,23 @@
         <v>0.90010000000000001</v>
       </c>
       <c r="AT15">
-        <f t="shared" ref="AT15:AT71" si="28">AQ15</f>
+        <f t="shared" ref="AT15:AT71" si="29">AQ15</f>
         <v>0.89269974336447477</v>
       </c>
       <c r="AU15">
-        <f t="shared" ref="AU15:AU71" si="29">AR15</f>
+        <f t="shared" ref="AU15:AU71" si="30">AR15</f>
         <v>0.90010000000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AW15">
+        <f t="shared" si="28"/>
+        <v>0.6</v>
+      </c>
+      <c r="AX15">
+        <f t="shared" si="28"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>2.5790999999999999</v>
       </c>
@@ -12603,15 +12514,23 @@
         <v>0.88049999999999995</v>
       </c>
       <c r="AT16">
+        <f t="shared" si="29"/>
+        <v>0.88768657134562523</v>
+      </c>
+      <c r="AU16">
+        <f t="shared" si="30"/>
+        <v>0.88049999999999995</v>
+      </c>
+      <c r="AW16">
         <f t="shared" si="28"/>
-        <v>0.88768657134562523</v>
-      </c>
-      <c r="AU16">
-        <f t="shared" si="29"/>
-        <v>0.88049999999999995</v>
-      </c>
-    </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.3">
+        <v>0.7</v>
+      </c>
+      <c r="AX16">
+        <f t="shared" si="28"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2.5750299999999999</v>
       </c>
@@ -12749,15 +12668,23 @@
         <v>0.88009999999999999</v>
       </c>
       <c r="AT17">
+        <f t="shared" si="29"/>
+        <v>0.8874729772413732</v>
+      </c>
+      <c r="AU17">
+        <f t="shared" si="30"/>
+        <v>0.88009999999999999</v>
+      </c>
+      <c r="AW17">
         <f t="shared" si="28"/>
-        <v>0.8874729772413732</v>
-      </c>
-      <c r="AU17">
-        <f t="shared" si="29"/>
-        <v>0.88009999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.3">
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="AX17">
+        <f t="shared" si="28"/>
+        <v>0.79999999999999993</v>
+      </c>
+    </row>
+    <row r="18" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>1.9464699999999999</v>
       </c>
@@ -12895,15 +12822,23 @@
         <v>0.82820000000000005</v>
       </c>
       <c r="AT18">
+        <f t="shared" si="29"/>
+        <v>0.82229479796580818</v>
+      </c>
+      <c r="AU18">
+        <f t="shared" si="30"/>
+        <v>0.82820000000000005</v>
+      </c>
+      <c r="AW18">
         <f t="shared" si="28"/>
-        <v>0.82229479796580818</v>
-      </c>
-      <c r="AU18">
-        <f t="shared" si="29"/>
-        <v>0.82820000000000005</v>
-      </c>
-    </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.3">
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="AX18">
+        <f t="shared" si="28"/>
+        <v>0.89999999999999991</v>
+      </c>
+    </row>
+    <row r="19" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>1.9030499999999999</v>
       </c>
@@ -13041,15 +12976,23 @@
         <v>0.82540000000000002</v>
       </c>
       <c r="AT19">
+        <f t="shared" si="29"/>
+        <v>0.81689658422107947</v>
+      </c>
+      <c r="AU19">
+        <f t="shared" si="30"/>
+        <v>0.82540000000000002</v>
+      </c>
+      <c r="AW19">
         <f t="shared" si="28"/>
-        <v>0.81689658422107947</v>
-      </c>
-      <c r="AU19">
-        <f t="shared" si="29"/>
-        <v>0.82540000000000002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.3">
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="AX19">
+        <f t="shared" si="28"/>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="20" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>1.2143600000000001</v>
       </c>
@@ -13187,15 +13130,23 @@
         <v>0.77990000000000004</v>
       </c>
       <c r="AT20">
+        <f t="shared" si="29"/>
+        <v>0.76660348734102246</v>
+      </c>
+      <c r="AU20">
+        <f t="shared" si="30"/>
+        <v>0.77990000000000004</v>
+      </c>
+      <c r="AW20">
         <f t="shared" si="28"/>
-        <v>0.76660348734102246</v>
-      </c>
-      <c r="AU20">
-        <f t="shared" si="29"/>
-        <v>0.77990000000000004</v>
-      </c>
-    </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.3">
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="AX20">
+        <f t="shared" si="28"/>
+        <v>1.0999999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>1.19438</v>
       </c>
@@ -13333,15 +13284,23 @@
         <v>0.78010000000000002</v>
       </c>
       <c r="AT21">
+        <f t="shared" si="29"/>
+        <v>0.76654455751265738</v>
+      </c>
+      <c r="AU21">
+        <f t="shared" si="30"/>
+        <v>0.78010000000000002</v>
+      </c>
+      <c r="AW21">
         <f t="shared" si="28"/>
-        <v>0.76654455751265738</v>
-      </c>
-      <c r="AU21">
-        <f t="shared" si="29"/>
-        <v>0.78010000000000002</v>
-      </c>
-    </row>
-    <row r="22" spans="1:47" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1.2</v>
+      </c>
+      <c r="AX21">
+        <f t="shared" si="28"/>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:50" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>1.16333</v>
       </c>
@@ -13479,15 +13438,23 @@
         <v>0.77749999999999997</v>
       </c>
       <c r="AT22">
+        <f t="shared" si="29"/>
+        <v>0.7665922051593731</v>
+      </c>
+      <c r="AU22">
+        <f t="shared" si="30"/>
+        <v>0.77749999999999997</v>
+      </c>
+      <c r="AW22">
         <f t="shared" si="28"/>
-        <v>0.7665922051593731</v>
-      </c>
-      <c r="AU22">
-        <f t="shared" si="29"/>
-        <v>0.77749999999999997</v>
-      </c>
-    </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.3">
+        <v>1.3</v>
+      </c>
+      <c r="AX22">
+        <f t="shared" si="28"/>
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>1.13737</v>
       </c>
@@ -13625,15 +13592,23 @@
         <v>0.77610000000000001</v>
       </c>
       <c r="AT23">
+        <f t="shared" si="29"/>
+        <v>0.76675134078691765</v>
+      </c>
+      <c r="AU23">
+        <f t="shared" si="30"/>
+        <v>0.77610000000000001</v>
+      </c>
+      <c r="AW23">
         <f t="shared" si="28"/>
-        <v>0.76675134078691765</v>
-      </c>
-      <c r="AU23">
-        <f t="shared" si="29"/>
-        <v>0.77610000000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.3">
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="AX23">
+        <f t="shared" si="28"/>
+        <v>1.4000000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>2.5646200000000001</v>
       </c>
@@ -13765,15 +13740,23 @@
         <v>0.87939999999999996</v>
       </c>
       <c r="AT24">
+        <f t="shared" si="29"/>
+        <v>0.88690839161497237</v>
+      </c>
+      <c r="AU24">
+        <f t="shared" si="30"/>
+        <v>0.87939999999999996</v>
+      </c>
+      <c r="AW24">
         <f t="shared" si="28"/>
-        <v>0.88690839161497237</v>
-      </c>
-      <c r="AU24">
-        <f t="shared" si="29"/>
-        <v>0.87939999999999996</v>
-      </c>
-    </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.3">
+        <v>1.5000000000000002</v>
+      </c>
+      <c r="AX24">
+        <f t="shared" si="28"/>
+        <v>1.5000000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>2.4317600000000001</v>
       </c>
@@ -13905,15 +13888,23 @@
         <v>0.86750000000000005</v>
       </c>
       <c r="AT25">
+        <f t="shared" si="29"/>
+        <v>0.8775556615512381</v>
+      </c>
+      <c r="AU25">
+        <f t="shared" si="30"/>
+        <v>0.86750000000000005</v>
+      </c>
+      <c r="AW25">
         <f t="shared" si="28"/>
-        <v>0.8775556615512381</v>
-      </c>
-      <c r="AU25">
-        <f t="shared" si="29"/>
-        <v>0.86750000000000005</v>
-      </c>
-    </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.3">
+        <v>1.6000000000000003</v>
+      </c>
+      <c r="AX25">
+        <f t="shared" si="28"/>
+        <v>1.6000000000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>2.2671299999999999</v>
       </c>
@@ -14045,15 +14036,23 @@
         <v>0.85389999999999999</v>
       </c>
       <c r="AT26">
+        <f t="shared" si="29"/>
+        <v>0.86138604864637769</v>
+      </c>
+      <c r="AU26">
+        <f t="shared" si="30"/>
+        <v>0.85389999999999999</v>
+      </c>
+      <c r="AW26">
         <f t="shared" si="28"/>
-        <v>0.86138604864637769</v>
-      </c>
-      <c r="AU26">
-        <f t="shared" si="29"/>
-        <v>0.85389999999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.3">
+        <v>1.7000000000000004</v>
+      </c>
+      <c r="AX26">
+        <f t="shared" si="28"/>
+        <v>1.7000000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>2.00387</v>
       </c>
@@ -14185,15 +14184,23 @@
         <v>0.83260000000000001</v>
       </c>
       <c r="AT27">
+        <f t="shared" si="29"/>
+        <v>0.82951849989245119</v>
+      </c>
+      <c r="AU27">
+        <f t="shared" si="30"/>
+        <v>0.83260000000000001</v>
+      </c>
+      <c r="AW27">
         <f t="shared" si="28"/>
-        <v>0.82951849989245119</v>
-      </c>
-      <c r="AU27">
-        <f t="shared" si="29"/>
-        <v>0.83260000000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.3">
+        <v>1.8000000000000005</v>
+      </c>
+      <c r="AX27">
+        <f t="shared" si="28"/>
+        <v>1.8000000000000005</v>
+      </c>
+    </row>
+    <row r="28" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>1.91442</v>
       </c>
@@ -14325,15 +14332,23 @@
         <v>0.82699999999999996</v>
       </c>
       <c r="AT28">
+        <f t="shared" si="29"/>
+        <v>0.81830195942847117</v>
+      </c>
+      <c r="AU28">
+        <f t="shared" si="30"/>
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="AW28">
         <f t="shared" si="28"/>
-        <v>0.81830195942847117</v>
-      </c>
-      <c r="AU28">
-        <f t="shared" si="29"/>
-        <v>0.82699999999999996</v>
-      </c>
-    </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.3">
+        <v>1.9000000000000006</v>
+      </c>
+      <c r="AX28">
+        <f t="shared" si="28"/>
+        <v>1.9000000000000006</v>
+      </c>
+    </row>
+    <row r="29" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>1.8589100000000001</v>
       </c>
@@ -14465,15 +14480,15 @@
         <v>0.8216</v>
       </c>
       <c r="AT29">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.81151350987312498</v>
       </c>
       <c r="AU29">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.8216</v>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>1.6414599999999999</v>
       </c>
@@ -14605,15 +14620,15 @@
         <v>0.80589999999999995</v>
       </c>
       <c r="AT30">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.78790497433784468</v>
       </c>
       <c r="AU30">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.80589999999999995</v>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>1.46208</v>
       </c>
@@ -14745,15 +14760,15 @@
         <v>0.79420000000000002</v>
       </c>
       <c r="AT31">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.77422135542550485</v>
       </c>
       <c r="AU31">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.79420000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>1.36084</v>
       </c>
@@ -14885,11 +14900,11 @@
         <v>0.78800000000000003</v>
       </c>
       <c r="AT32">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.76949093861106632</v>
       </c>
       <c r="AU32">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.78800000000000003</v>
       </c>
     </row>
@@ -15025,11 +15040,11 @@
         <v>0.78090000000000004</v>
       </c>
       <c r="AT33">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.76671883473819458</v>
       </c>
       <c r="AU33">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.78090000000000004</v>
       </c>
     </row>
@@ -15165,11 +15180,11 @@
         <v>0.77569999999999995</v>
       </c>
       <c r="AT34">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.76712830800820742</v>
       </c>
       <c r="AU34">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.77569999999999995</v>
       </c>
     </row>
@@ -15305,11 +15320,11 @@
         <v>0.76890000000000003</v>
       </c>
       <c r="AT35">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.76941183907369515</v>
       </c>
       <c r="AU35">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.76890000000000003</v>
       </c>
     </row>
@@ -15445,11 +15460,11 @@
         <v>0.76590000000000003</v>
       </c>
       <c r="AT36">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.77076499395109788</v>
       </c>
       <c r="AU36">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.76590000000000003</v>
       </c>
     </row>
@@ -15585,11 +15600,11 @@
         <v>0.76500000000000001</v>
       </c>
       <c r="AT37">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.77091774416082515</v>
       </c>
       <c r="AU37">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.76500000000000001</v>
       </c>
     </row>
@@ -15725,11 +15740,11 @@
         <v>0.78820000000000001</v>
       </c>
       <c r="AT38">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.7846116597075965</v>
       </c>
       <c r="AU38">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.78820000000000001</v>
       </c>
     </row>
@@ -15865,11 +15880,11 @@
         <v>0.78749999999999998</v>
       </c>
       <c r="AT39">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.78419607343218001</v>
       </c>
       <c r="AU39">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.78749999999999998</v>
       </c>
     </row>
@@ -16005,11 +16020,11 @@
         <v>0.78600000000000003</v>
       </c>
       <c r="AT40">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.78138986523727028</v>
       </c>
       <c r="AU40">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.78600000000000003</v>
       </c>
     </row>
@@ -16145,11 +16160,11 @@
         <v>0.78490000000000004</v>
       </c>
       <c r="AT41">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.77639766769479412</v>
       </c>
       <c r="AU41">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.78490000000000004</v>
       </c>
     </row>
@@ -16285,11 +16300,11 @@
         <v>0.78359999999999996</v>
       </c>
       <c r="AT42">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.76670543121302348</v>
       </c>
       <c r="AU42">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.78359999999999996</v>
       </c>
     </row>
@@ -17481,11 +17496,11 @@
         <v>0.93899999999999995</v>
       </c>
       <c r="AT51">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.94335378750288057</v>
       </c>
       <c r="AU51">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.93899999999999995</v>
       </c>
     </row>
@@ -17621,11 +17636,11 @@
         <v>0.92849999999999999</v>
       </c>
       <c r="AT52">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.9351871899641544</v>
       </c>
       <c r="AU52">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.92849999999999999</v>
       </c>
     </row>
@@ -17761,11 +17776,11 @@
         <v>0.86890000000000001</v>
       </c>
       <c r="AT53">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.86285132061673442</v>
       </c>
       <c r="AU53">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.86890000000000001</v>
       </c>
     </row>
@@ -17901,11 +17916,11 @@
         <v>0.83320000000000005</v>
       </c>
       <c r="AT54">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.81370847574829164</v>
       </c>
       <c r="AU54">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.83320000000000005</v>
       </c>
     </row>
@@ -18041,11 +18056,11 @@
         <v>0.8115</v>
       </c>
       <c r="AT55">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.7939055308345776</v>
       </c>
       <c r="AU55">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.8115</v>
       </c>
     </row>
@@ -18181,11 +18196,11 @@
         <v>0.80889999999999995</v>
       </c>
       <c r="AT56">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.7922437943155205</v>
       </c>
       <c r="AU56">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.80889999999999995</v>
       </c>
     </row>
@@ -18321,11 +18336,11 @@
         <v>0.79159999999999997</v>
       </c>
       <c r="AT57">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.78695351560083271</v>
       </c>
       <c r="AU57">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.79159999999999997</v>
       </c>
     </row>
@@ -18461,11 +18476,11 @@
         <v>0.7893</v>
       </c>
       <c r="AT58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.78673362074081621</v>
       </c>
       <c r="AU58">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.7893</v>
       </c>
     </row>
@@ -18601,11 +18616,11 @@
         <v>0.7843</v>
       </c>
       <c r="AT59">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.7854911290820068</v>
       </c>
       <c r="AU59">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.7843</v>
       </c>
     </row>
@@ -18741,11 +18756,11 @@
         <v>0.76339999999999997</v>
       </c>
       <c r="AT60">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.78820296142452151</v>
       </c>
       <c r="AU60">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.76339999999999997</v>
       </c>
     </row>
@@ -18881,11 +18896,11 @@
         <v>0.76170000000000004</v>
       </c>
       <c r="AT61">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.78789735467023703</v>
       </c>
       <c r="AU61">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.76170000000000004</v>
       </c>
     </row>
@@ -19021,11 +19036,11 @@
         <v>0.96289999999999998</v>
       </c>
       <c r="AT62">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.95441741296299187</v>
       </c>
       <c r="AU62">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.96289999999999998</v>
       </c>
     </row>
@@ -19161,11 +19176,11 @@
         <v>0.96060000000000001</v>
       </c>
       <c r="AT63">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.9541114117243763</v>
       </c>
       <c r="AU63">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.96060000000000001</v>
       </c>
     </row>
@@ -19301,11 +19316,11 @@
         <v>0.9476</v>
       </c>
       <c r="AT64">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.95050719221639624</v>
       </c>
       <c r="AU64">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.9476</v>
       </c>
     </row>
@@ -19441,11 +19456,11 @@
         <v>0.91900000000000004</v>
       </c>
       <c r="AT65">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.93119761989592975</v>
       </c>
       <c r="AU65">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.91900000000000004</v>
       </c>
     </row>
@@ -19581,11 +19596,11 @@
         <v>0.89790000000000003</v>
       </c>
       <c r="AT66">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.90823729269878817</v>
       </c>
       <c r="AU66">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.89790000000000003</v>
       </c>
     </row>
@@ -19721,11 +19736,11 @@
         <v>0.88390000000000002</v>
       </c>
       <c r="AT67">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.88988525809747077</v>
       </c>
       <c r="AU67">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.88390000000000002</v>
       </c>
     </row>
@@ -19861,11 +19876,11 @@
         <v>0.83340000000000003</v>
       </c>
       <c r="AT68">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.8181181367341841</v>
       </c>
       <c r="AU68">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.83340000000000003</v>
       </c>
     </row>
@@ -20001,11 +20016,11 @@
         <v>0.79690000000000005</v>
       </c>
       <c r="AT69">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.78844742641251309</v>
       </c>
       <c r="AU69">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.79690000000000005</v>
       </c>
     </row>
@@ -20141,11 +20156,11 @@
         <v>0.7823</v>
       </c>
       <c r="AT70">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.78558276910401126</v>
       </c>
       <c r="AU70">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.7823</v>
       </c>
     </row>
@@ -20234,7 +20249,7 @@
         <v>3222.7493614805044</v>
       </c>
       <c r="AA71">
-        <f t="shared" ref="AA71" si="30">D71/(1000+D71)</f>
+        <f t="shared" ref="AA71" si="31">D71/(1000+D71)</f>
         <v>7.2223947052743986E-2</v>
       </c>
       <c r="AB71">
@@ -20262,7 +20277,7 @@
         <v>-47.750139079775813</v>
       </c>
       <c r="AM71">
-        <f t="shared" ref="AM71" si="31">(Q71-U71)+X71-AC71-AK71</f>
+        <f t="shared" ref="AM71" si="32">(Q71-U71)+X71-AC71-AK71</f>
         <v>-29.758326428987253</v>
       </c>
       <c r="AN71" s="1">
@@ -20281,11 +20296,11 @@
         <v>0.77590000000000003</v>
       </c>
       <c r="AT71">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.77827380953468461</v>
       </c>
       <c r="AU71">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.77590000000000003</v>
       </c>
     </row>
@@ -21358,8 +21373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAA53125-8324-42F8-BF4C-83E8BB87300B}">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21399,12 +21414,6 @@
       <c r="B3" s="1">
         <v>271.77023032931601</v>
       </c>
-      <c r="D3">
-        <v>0.13125400000000001</v>
-      </c>
-      <c r="E3">
-        <v>259</v>
-      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -21413,12 +21422,6 @@
       <c r="B4" s="1">
         <v>270.10528340824402</v>
       </c>
-      <c r="D4">
-        <v>8.5834900000000006E-2</v>
-      </c>
-      <c r="E4">
-        <v>260</v>
-      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -21427,12 +21430,6 @@
       <c r="B5" s="1">
         <v>268.44208538099599</v>
       </c>
-      <c r="D5">
-        <v>0.14215900000000001</v>
-      </c>
-      <c r="E5">
-        <v>261</v>
-      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -21441,12 +21438,6 @@
       <c r="B6" s="1">
         <v>267.91479389286201</v>
       </c>
-      <c r="D6">
-        <v>0.14127400000000001</v>
-      </c>
-      <c r="E6">
-        <v>262</v>
-      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -21469,12 +21460,6 @@
       <c r="B8" s="1">
         <v>260.064009513982</v>
       </c>
-      <c r="D8">
-        <v>0.13661799999999999</v>
-      </c>
-      <c r="E8">
-        <v>264</v>
-      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -21482,12 +21467,6 @@
       </c>
       <c r="B9" s="1">
         <v>254.423826929467</v>
-      </c>
-      <c r="D9">
-        <v>2.6268300000000001E-2</v>
-      </c>
-      <c r="E9">
-        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -22290,20 +22269,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="49fa8af8-517d-491f-a3d5-7cf68fb985f9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="49fa8af8-517d-491f-a3d5-7cf68fb985f9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22326,14 +22305,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71225005-2353-48CA-B97F-AA326ECE473F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{715EA469-2506-458C-8899-792543708004}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -22348,4 +22319,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71225005-2353-48CA-B97F-AA326ECE473F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>